<commit_message>
Update datasets used for vignettes
</commit_message>
<xml_diff>
--- a/vignettes/s_pneumoniae_strains_sweden.xlsx
+++ b/vignettes/s_pneumoniae_strains_sweden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholascroucher/Documents/progression_rate_estimation/progressionEstimation/vignettes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FE13DE-8B84-6C48-A8B9-16096C067BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93E3521-0D4D-4147-A6A2-8F4F35CA8053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32340" yWindow="3880" windowWidth="31340" windowHeight="14440" xr2:uid="{68B6CDF4-21FC-164B-AD92-181213EE6C3E}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E2" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,6 +506,7 @@
         <v>0</v>
       </c>
       <c r="E2">
+        <f>611+719</f>
         <v>1330</v>
       </c>
       <c r="F2">
@@ -532,6 +533,7 @@
         <v>3</v>
       </c>
       <c r="E3">
+        <f t="shared" ref="E3:E19" si="0">611+719</f>
         <v>1330</v>
       </c>
       <c r="F3">
@@ -558,6 +560,7 @@
         <v>0</v>
       </c>
       <c r="E4">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F4">
@@ -584,6 +587,7 @@
         <v>0</v>
       </c>
       <c r="E5">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F5">
@@ -610,6 +614,7 @@
         <v>2</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F6">
@@ -636,6 +641,7 @@
         <v>0</v>
       </c>
       <c r="E7">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F7">
@@ -662,6 +668,7 @@
         <v>12</v>
       </c>
       <c r="E8">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F8">
@@ -688,6 +695,7 @@
         <v>7</v>
       </c>
       <c r="E9">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F9">
@@ -714,6 +722,7 @@
         <v>9</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F10">
@@ -740,6 +749,7 @@
         <v>13</v>
       </c>
       <c r="E11">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F11">
@@ -766,6 +776,7 @@
         <v>0</v>
       </c>
       <c r="E12">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F12">
@@ -792,6 +803,7 @@
         <v>10</v>
       </c>
       <c r="E13">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F13">
@@ -818,6 +830,7 @@
         <v>2</v>
       </c>
       <c r="E14">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F14">
@@ -844,6 +857,7 @@
         <v>4</v>
       </c>
       <c r="E15">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F15">
@@ -870,6 +884,7 @@
         <v>1</v>
       </c>
       <c r="E16">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F16">
@@ -896,6 +911,7 @@
         <v>0</v>
       </c>
       <c r="E17">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F17">
@@ -922,6 +938,7 @@
         <v>0</v>
       </c>
       <c r="E18">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F18">
@@ -948,6 +965,7 @@
         <v>2</v>
       </c>
       <c r="E19">
+        <f t="shared" si="0"/>
         <v>1330</v>
       </c>
       <c r="F19">
@@ -988,10 +1006,10 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="carriage_samples" prompt="The number of individuals in the carriage study, including negative samples (must be a non-negative integer that is consistent across each study)" sqref="E20:E1048576 D11:D19 C2:C10 E1" xr:uid="{08AFE457-53F4-3344-ADAD-98B6ABDF6FDA}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="surveillance_population" prompt="The number of individuals of the relevant demographic in the population under surveillance (must be a non-negative integer consistent across each study)" sqref="F20:F1048576 E11:E19 D2:D10 F1" xr:uid="{26AFF274-CC83-2247-99E6-36F14F832043}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="surveillance_population" prompt="The number of individuals of the relevant demographic in the population under surveillance (must be a non-negative integer consistent across each study)" sqref="F20:F1048576 F1 D2:D10" xr:uid="{26AFF274-CC83-2247-99E6-36F14F832043}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="time_interval" prompt="The duration of the disease surveillance period (must be consistent across each study)" sqref="G20:G1048576 F11:F19 E2:E10 G1" xr:uid="{7D5C3DA2-22EC-F746-AB8E-DFE0F6C2EECB}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="time_interval" prompt="The duration of the disease surveillance period (must be consistent across each study)" sqref="G20:G1048576 F11:F19 G1 E2:E19" xr:uid="{7D5C3DA2-22EC-F746-AB8E-DFE0F6C2EECB}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="strain" prompt="Optional column specifying the strain background when two subtyping categoriations are used in the analysis" sqref="H20:H1048576 G11:G19 F2:F10 H1" xr:uid="{EEEAAE33-77E6-8947-BE6B-00538FD9F9CA}"/>

</xml_diff>